<commit_message>
change Patrick Toole III to Patrick III Toole for better matching
</commit_message>
<xml_diff>
--- a/Dining.xlsx
+++ b/Dining.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrysterling/Documents/Python/Disney/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFF87A4-E98C-A34D-9F7E-80F6F037E80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9156B3D5-8952-5C48-8B6D-2A692228A6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31900" yWindow="-860" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,9 +98,6 @@
     <t>Sean Nayden</t>
   </si>
   <si>
-    <t>Patrick Toole II</t>
-  </si>
-  <si>
     <t>Jackie Knotts</t>
   </si>
   <si>
@@ -110,33 +107,18 @@
     <t>Robby Toole</t>
   </si>
   <si>
-    <t>Sean Nayden,Harrison Nayden,Brianne Sterling,Harry Sterling,Patrick Toole III</t>
-  </si>
-  <si>
-    <t>Grandpa,Patrick Toole III,Brianne Sterling,Harry Sterling,Sabrina Quigley,Will Quigley</t>
-  </si>
-  <si>
     <t>Sean Nayden,Harrison Nayden,Lexi Knotts,Jackie Knotts,Grandpa,Grandma</t>
   </si>
   <si>
-    <t>Patrick Toole II,Lyndy Toole</t>
-  </si>
-  <si>
     <t>Sabrina Quigley,Will Quigley</t>
   </si>
   <si>
-    <t>Sean Nayden,Harrison Nayden,Patrick Toole II,Lyndy Toole,Lexi Knotts</t>
-  </si>
-  <si>
     <t>Jackie Knotts,Grandma,Grandpa,Lexi Knotts</t>
   </si>
   <si>
     <t>Grandpa,Grandma,Jackie Knotts,Lexi Knotts</t>
   </si>
   <si>
-    <t>Robby Toole,Andre Toole,Max Toole,Gussie Toole,Patrick Toole II,Lyndy Toole</t>
-  </si>
-  <si>
     <t>Sabrina Quigley</t>
   </si>
   <si>
@@ -161,9 +143,6 @@
     <t>Joe Schifano</t>
   </si>
   <si>
-    <t>Robby Toole,Andre Toole,Gussie Toole,Max Toole,Lexi Knotts,Patrick Toole II</t>
-  </si>
-  <si>
     <t>Lexi Knotts,Elizabeth James,Anthony Lester,Vinne Lester,Max Toole,Gussie Toole</t>
   </si>
   <si>
@@ -182,9 +161,6 @@
     <t>Chris Paroby</t>
   </si>
   <si>
-    <t>Lyndy Toole,Patrick Toole II,Sabrina Quigley,Chris Paroby,Marie Mazzoni</t>
-  </si>
-  <si>
     <t>Grandma,Grandpa,Stephen Paroby,Chris Paroby,Jackie Knotts</t>
   </si>
   <si>
@@ -194,28 +170,52 @@
     <t>Chris Paroby,Stephen Paroby,Jacob Paroby,Grandma,Lyndy Toole</t>
   </si>
   <si>
-    <t>Sean Nayden,Harrison Nayden,Grandpa,Patrick Toole III,Andre Toole,Robby Toole</t>
-  </si>
-  <si>
-    <t>Chris Paroby,Stephen Paroby,Jacob Paroby,Patrick Toole III,Grandpa,Grandma</t>
-  </si>
-  <si>
-    <t>Robby Toole,Andre Toole,Lyndy Toole,Patrick Toole III,Patrick Toole II</t>
-  </si>
-  <si>
     <t>Lexi Knotts,Elizabeth James,Ashley James,Anthony Lester,Max Toole,Gussie Toole</t>
   </si>
   <si>
     <t>Sabrina Quigley,Will Quigley,Sean Nayden,Harrison Nayden,Lexi Knotts</t>
   </si>
   <si>
-    <t>Robby Toole,Andre Toole,Patrick Toole II,Lyndy Toole,Nicole James</t>
-  </si>
-  <si>
     <t>Kelly O'Connor,Jackie Knotts,Natalie Lester,Grandma,Nicole James,Brianne Sterling</t>
   </si>
   <si>
     <t>Brianne Sterling,Harry Sterling,Natalie Lester,Marie Mazzoni,Dick Mazzoni</t>
+  </si>
+  <si>
+    <t>Sean Nayden,Harrison Nayden,Brianne Sterling,Harry Sterling,Patrick III Toole</t>
+  </si>
+  <si>
+    <t>Grandpa,Patrick III Toole,Brianne Sterling,Harry Sterling,Sabrina Quigley,Will Quigley</t>
+  </si>
+  <si>
+    <t>Sean Nayden,Harrison Nayden,Grandpa,Patrick III Toole,Andre Toole,Robby Toole</t>
+  </si>
+  <si>
+    <t>Chris Paroby,Stephen Paroby,Jacob Paroby,Patrick III Toole,Grandpa,Grandma</t>
+  </si>
+  <si>
+    <t>Robby Toole,Andre Toole,Max Toole,Gussie Toole,Patrick II Toole,Lyndy Toole</t>
+  </si>
+  <si>
+    <t>Patrick II Toole</t>
+  </si>
+  <si>
+    <t>Patrick II Toole,Lyndy Toole</t>
+  </si>
+  <si>
+    <t>Sean Nayden,Harrison Nayden,Patrick II Toole,Lyndy Toole,Lexi Knotts</t>
+  </si>
+  <si>
+    <t>Robby Toole,Andre Toole,Lyndy Toole,Patrick III Toole,Patrick II Toole</t>
+  </si>
+  <si>
+    <t>Robby Toole,Andre Toole,Gussie Toole,Max Toole,Lexi Knotts,Patrick II Toole</t>
+  </si>
+  <si>
+    <t>Lyndy Toole,Patrick II Toole,Sabrina Quigley,Chris Paroby,Marie Mazzoni</t>
+  </si>
+  <si>
+    <t>Robby Toole,Andre Toole,Patrick II Toole,Lyndy Toole,Nicole James</t>
   </si>
 </sst>
 </file>
@@ -223,8 +223,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -264,10 +264,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,7 +486,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -529,7 +529,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -546,7 +546,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -560,10 +560,10 @@
         <v>0.75347222222222221</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -580,7 +580,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -597,7 +597,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -611,10 +611,10 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -631,7 +631,7 @@
         <v>19</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -645,10 +645,10 @@
         <v>0.79861111111111116</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -662,10 +662,10 @@
         <v>0.75</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -682,7 +682,7 @@
         <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -696,10 +696,10 @@
         <v>0.75</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -716,7 +716,7 @@
         <v>17</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -730,10 +730,10 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
@@ -750,7 +750,7 @@
         <v>19</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
@@ -767,7 +767,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
@@ -784,7 +784,7 @@
         <v>19</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
@@ -798,10 +798,10 @@
         <v>0.36458333333333331</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
@@ -818,7 +818,7 @@
         <v>17</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
@@ -832,10 +832,10 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
@@ -849,10 +849,10 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
@@ -866,10 +866,10 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
@@ -883,10 +883,10 @@
         <v>0.73263888888888884</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
@@ -900,10 +900,10 @@
         <v>0.37152777777777773</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
@@ -917,10 +917,10 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
@@ -934,10 +934,10 @@
         <v>0.75694444444444453</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
@@ -951,10 +951,10 @@
         <v>0.74652777777777779</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
@@ -968,10 +968,10 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
@@ -985,10 +985,10 @@
         <v>0.375</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
@@ -1002,10 +1002,10 @@
         <v>0.77777777777777779</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
@@ -1019,10 +1019,10 @@
         <v>0.74652777777777779</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>